<commit_message>
Included Jira ID's for each test case data.
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/Transmittals-Fluid-Navigation.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/Transmittals-Fluid-Navigation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Home</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>FluidTx7_Menu3</t>
+  </si>
+  <si>
+    <t>RefID</t>
+  </si>
+  <si>
+    <t>LATFLD-2</t>
   </si>
 </sst>
 </file>
@@ -466,127 +472,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="25.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="3" width="25.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:17">
+      <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="str">
-        <f>C2</f>
+      <c r="G2" s="1" t="str">
+        <f>D2</f>
         <v>Home</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated the FluidTX column names from FluidTx7 to FluidTx as per update constant for appName
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/Transmittals-Fluid-Navigation.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/Transmittals-Fluid-Navigation.xlsx
@@ -94,22 +94,22 @@
     <t>11</t>
   </si>
   <si>
-    <t>FluidTx7_MenuCount</t>
-  </si>
-  <si>
-    <t>FluidTx7_Menu1</t>
-  </si>
-  <si>
-    <t>FluidTx7_Menu2</t>
-  </si>
-  <si>
-    <t>FluidTx7_Menu3</t>
-  </si>
-  <si>
     <t>RefID</t>
   </si>
   <si>
     <t>LATFLD-2</t>
+  </si>
+  <si>
+    <t>FluidTx_MenuCount</t>
+  </si>
+  <si>
+    <t>FluidTx_Menu1</t>
+  </si>
+  <si>
+    <t>FluidTx_Menu2</t>
+  </si>
+  <si>
+    <t>FluidTx_Menu3</t>
   </si>
 </sst>
 </file>
@@ -474,9 +474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -500,22 +498,22 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>7</v>
@@ -553,7 +551,7 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>

</xml_diff>